<commit_message>
ownership data and house prices update
</commit_message>
<xml_diff>
--- a/data/raw/ownership.xlsx
+++ b/data/raw/ownership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marten/Documents/projects/inequality/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABACFAE-89B8-9249-A2E2-2A9F7DAE4479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791B24CB-6B27-A147-9EA5-C92A0A442F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12800" windowHeight="15500" xr2:uid="{A244A359-7D9D-9D45-9DFD-36A583F98E88}"/>
   </bookViews>
@@ -36,11 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
-  <si>
-    <t>euro
-area</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>BE</t>
   </si>
@@ -130,6 +126,12 @@
   </si>
   <si>
     <t>LT</t>
+  </si>
+  <si>
+    <t>I9</t>
+  </si>
+  <si>
+    <t>Decile</t>
   </si>
 </sst>
 </file>
@@ -558,96 +560,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE5B78B-1E8A-8447-A059-64CCFB2940B5}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="29" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2">
         <v>2014</v>
@@ -721,7 +723,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>2014</v>
@@ -795,7 +797,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>2014</v>
@@ -869,7 +871,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <v>2014</v>
@@ -943,7 +945,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2">
         <v>2014</v>
@@ -1017,7 +1019,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <v>2014</v>
@@ -1091,7 +1093,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <v>2021</v>
@@ -1168,7 +1170,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>2021</v>
@@ -1245,7 +1247,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>2021</v>
@@ -1322,7 +1324,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <v>2021</v>
@@ -1399,7 +1401,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
         <v>2021</v>
@@ -1476,7 +1478,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
         <v>2021</v>

</xml_diff>